<commit_message>
[CPU] SCH, test data update
</commit_message>
<xml_diff>
--- a/1_Schematic/Build V2.0/RF-GEN-Change list_20200127.xlsx
+++ b/1_Schematic/Build V2.0/RF-GEN-Change list_20200127.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Issue list" sheetId="2" r:id="rId1"/>
@@ -17,190 +17,190 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="77">
   <si>
     <t>No</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Reference</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Sheet</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Before</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>After</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Description</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Applied Date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>RF Generator - CPU V1.0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>No</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PCB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>CPU</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>OPEN</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Issue</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>U4 feedback path에 CAP 필요</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Description</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>수정 사항</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>U4의 Gain이 5.3이상 증가하지 않음</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>R20을 1K-&gt; 806으로 조정해도 Gain이 0.2만 상승함(계산치 1이상임)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>기존 회로</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Jumpper 필요</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>V2.0 SCH, PCB 수정</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>RF Gen Issue list</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Version</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>v1.0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>SCH</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PCB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>BOM</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>HD1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Top 배치</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Bottom 배치 Library</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>HEADER PIN과 PCB Library 구별</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>C69</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2.2uF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>RF signal만 증폭시키기 위해 Feedback Path에 Bypass CAP 필요함</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>RF signal만 증폭시키기 위해 Feedback Path에 Bypass CAP</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>2/5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>RF Generator - PWR V1.0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>F1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PCB Library miss - Hole</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>HOLE - circle</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>HOLE - 장홀</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>HD1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>HIF3H-20PA-2.54DSA</t>
@@ -210,55 +210,139 @@
   </si>
   <si>
     <t>PN Miss 수정</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>-</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>PWR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>v1.0</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>L4 Core size 확대</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>발열 개선을 위해 큰 size 사용</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Closed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>RF</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Heat Sink FET Hole 위치 miss</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Top view로 작성하여 Mirror 되어 있음</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CPU</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>v2.0</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>R67 value miss</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>PL의 V_PN, V_Desc 오기</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RC5025FR15</t>
+  </si>
+  <si>
+    <t>R67</t>
+  </si>
+  <si>
+    <t>PL의 V_PN, V_Desc 오기 수정</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>RC5025F101CS</t>
+  </si>
+  <si>
+    <t>ST-LINK connection error</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>JNTRST Pull-up NC 처리 후 정상 동작</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Closed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>R6, R7, R9</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>10K</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>NC</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ST-LINK Connection error</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2/7</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>JTAG1 Pin-map과 DL JIG pin-map miss match</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">DL JIG에서 CON를 Bottom Solder </t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
+  </numFmts>
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -438,6 +522,14 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -632,7 +724,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1027,58 +1119,187 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1087,10 +1308,7 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1099,10 +1317,7 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1111,10 +1326,7 @@
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1123,10 +1335,7 @@
     <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1135,10 +1344,7 @@
     <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1147,41 +1353,11 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1189,7 +1365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1219,31 +1395,31 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1254,78 +1430,114 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="1" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="34" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="1" xfId="51" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="34" borderId="9" xfId="51" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="34" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="34" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="1" xfId="41" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="1" xfId="51" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="71">
     <cellStyle name="20% - 강조색1" xfId="18" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색1 2" xfId="53"/>
     <cellStyle name="20% - 강조색2" xfId="22" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색2 2" xfId="56"/>
     <cellStyle name="20% - 강조색3" xfId="26" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색3 2" xfId="59"/>
     <cellStyle name="20% - 강조색4" xfId="30" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색4 2" xfId="62"/>
     <cellStyle name="20% - 강조색5" xfId="34" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색5 2" xfId="65"/>
     <cellStyle name="20% - 강조색6" xfId="38" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="20% - 강조색6 2" xfId="68"/>
     <cellStyle name="40% - 강조색1" xfId="19" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색1 2" xfId="54"/>
     <cellStyle name="40% - 강조색2" xfId="23" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색2 2" xfId="57"/>
     <cellStyle name="40% - 강조색3" xfId="27" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색3 2" xfId="60"/>
     <cellStyle name="40% - 강조색4" xfId="31" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색4 2" xfId="63"/>
     <cellStyle name="40% - 강조색5" xfId="35" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색5 2" xfId="66"/>
     <cellStyle name="40% - 강조색6" xfId="39" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="40% - 강조색6 2" xfId="69"/>
     <cellStyle name="60% - 강조색1" xfId="20" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - 강조색1 2" xfId="45"/>
+    <cellStyle name="60% - 강조색1 3" xfId="55"/>
     <cellStyle name="60% - 강조색2" xfId="24" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - 강조색2 2" xfId="46"/>
+    <cellStyle name="60% - 강조색2 3" xfId="58"/>
     <cellStyle name="60% - 강조색3" xfId="28" builtinId="40" customBuiltin="1"/>
     <cellStyle name="60% - 강조색3 2" xfId="47"/>
+    <cellStyle name="60% - 강조색3 3" xfId="61"/>
     <cellStyle name="60% - 강조색4" xfId="32" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - 강조색4 2" xfId="48"/>
+    <cellStyle name="60% - 강조색4 3" xfId="64"/>
     <cellStyle name="60% - 강조색5" xfId="36" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - 강조색5 2" xfId="49"/>
+    <cellStyle name="60% - 강조색5 3" xfId="67"/>
     <cellStyle name="60% - 강조색6" xfId="40" builtinId="52" customBuiltin="1"/>
     <cellStyle name="60% - 강조색6 2" xfId="50"/>
+    <cellStyle name="60% - 강조색6 3" xfId="70"/>
     <cellStyle name="강조색1" xfId="17" builtinId="29" customBuiltin="1"/>
     <cellStyle name="강조색2" xfId="21" builtinId="33" customBuiltin="1"/>
     <cellStyle name="강조색3" xfId="25" builtinId="37" customBuiltin="1"/>
@@ -1336,6 +1548,7 @@
     <cellStyle name="계산" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="나쁨" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="메모 2" xfId="42"/>
+    <cellStyle name="메모 3" xfId="52"/>
     <cellStyle name="보통" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="보통 2" xfId="44"/>
     <cellStyle name="설명 텍스트" xfId="15" builtinId="53" customBuiltin="1"/>
@@ -1353,6 +1566,7 @@
     <cellStyle name="출력" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="표준 2" xfId="41"/>
+    <cellStyle name="표준 3" xfId="51"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1653,8 +1867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1663,7 +1877,7 @@
     <col min="2" max="2" width="5.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="9" style="2"/>
-    <col min="7" max="7" width="33.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43.875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="62.25" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.75" style="1" customWidth="1"/>
     <col min="10" max="10" width="19.125" style="1" bestFit="1" customWidth="1"/>
@@ -1709,28 +1923,28 @@
       <c r="B5" s="24">
         <v>1</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="36">
         <v>43857</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="30" t="s">
+      <c r="J5" s="29" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1795,7 +2009,7 @@
         <v>55</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>13</v>
@@ -1810,40 +2024,80 @@
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
+      <c r="B9" s="30">
+        <v>5</v>
+      </c>
+      <c r="C9" s="40">
+        <v>43868</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="31"/>
+      <c r="J9" s="35"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="7"/>
+      <c r="B10" s="30">
+        <v>6</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="31"/>
+      <c r="J10" s="35"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7"/>
+      <c r="B11" s="30">
+        <v>7</v>
+      </c>
+      <c r="C11" s="39"/>
+      <c r="D11" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="31"/>
+      <c r="J11" s="35"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
       <c r="C12" s="12"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1854,7 +2108,9 @@
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
+      <c r="B13" s="4">
+        <v>9</v>
+      </c>
       <c r="C13" s="12"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
@@ -1865,7 +2121,9 @@
       <c r="J13" s="7"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
+      <c r="B14" s="4">
+        <v>10</v>
+      </c>
       <c r="C14" s="12"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1876,7 +2134,9 @@
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="4"/>
+      <c r="B15" s="4">
+        <v>11</v>
+      </c>
       <c r="C15" s="12"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1887,7 +2147,9 @@
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="4"/>
+      <c r="B16" s="4">
+        <v>12</v>
+      </c>
       <c r="C16" s="12"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1898,7 +2160,9 @@
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="4"/>
+      <c r="B17" s="4">
+        <v>13</v>
+      </c>
       <c r="C17" s="12"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -1909,7 +2173,9 @@
       <c r="J17" s="7"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="4"/>
+      <c r="B18" s="4">
+        <v>14</v>
+      </c>
       <c r="C18" s="12"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
@@ -1920,7 +2186,9 @@
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="4"/>
+      <c r="B19" s="4">
+        <v>15</v>
+      </c>
       <c r="C19" s="6"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
@@ -1931,7 +2199,9 @@
       <c r="J19" s="7"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="4"/>
+      <c r="B20" s="4">
+        <v>16</v>
+      </c>
       <c r="C20" s="6"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -1975,7 +2245,10 @@
       <c r="J23" s="11"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <mergeCells count="1">
+    <mergeCell ref="C9:C11"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -1986,7 +2259,7 @@
   <dimension ref="B2:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2049,95 +2322,129 @@
       <c r="B5" s="24">
         <v>1</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="38">
         <v>43866</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>6</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="30"/>
+      <c r="L5" s="29"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="31">
+      <c r="B6" s="30">
         <v>2</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33">
+      <c r="C6" s="39"/>
+      <c r="D6" s="31">
         <v>2</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="33" t="s">
+      <c r="G6" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I6" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="36" t="s">
+      <c r="K6" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="37"/>
+      <c r="L6" s="35"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="4">
+      <c r="B7" s="30">
         <v>3</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="7"/>
+      <c r="C7" s="40">
+        <v>43868</v>
+      </c>
+      <c r="D7" s="31">
+        <v>5</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="L7" s="35"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="4">
+      <c r="B8" s="30">
         <v>4</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="7"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="31">
+        <v>1</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="K8" s="43" t="s">
+        <v>73</v>
+      </c>
+      <c r="L8" s="35"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
@@ -2149,9 +2456,9 @@
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -2164,9 +2471,9 @@
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
@@ -2179,9 +2486,9 @@
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
@@ -2194,9 +2501,9 @@
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
       <c r="L12" s="7"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
@@ -2209,9 +2516,9 @@
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
       <c r="L13" s="7"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
@@ -2224,9 +2531,9 @@
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
@@ -2239,9 +2546,9 @@
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
       <c r="L15" s="7"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
@@ -2254,9 +2561,9 @@
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
       <c r="L16" s="7"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
@@ -2269,9 +2576,9 @@
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
       <c r="L17" s="7"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
@@ -2284,9 +2591,9 @@
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
       <c r="L18" s="7"/>
     </row>
     <row r="19" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2299,16 +2606,17 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
       <c r="L19" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -2318,8 +2626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2382,65 +2690,65 @@
       <c r="B5" s="24">
         <v>1</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="38">
         <v>43866</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="25">
         <v>3</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="29" t="s">
+      <c r="I5" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="29" t="s">
+      <c r="K5" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="L5" s="30"/>
+      <c r="L5" s="29"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="31">
+      <c r="B6" s="30">
         <v>2</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="33">
+      <c r="C6" s="39"/>
+      <c r="D6" s="31">
         <v>4</v>
       </c>
-      <c r="E6" s="34" t="s">
+      <c r="E6" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F6" s="34" t="s">
+      <c r="F6" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="I6" s="36" t="s">
+      <c r="I6" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="36" t="s">
+      <c r="J6" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="K6" s="36" t="s">
+      <c r="K6" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="37"/>
+      <c r="L6" s="35"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
@@ -2641,7 +2949,7 @@
   <mergeCells count="1">
     <mergeCell ref="C5:C6"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -2655,7 +2963,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>